<commit_message>
* A first version of function to obtain a Graph of All information available in the State of a case study, using NetworkX * Some refactorizations
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/Soslaires.xlsx
+++ b/backend_tests/z_input_files/Soslaires.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="D13" authorId="0">
@@ -365,16 +365,16 @@
     <t xml:space="preserve">MW</t>
   </si>
   <si>
-    <t xml:space="preserve">LU.cost</t>
+    <t xml:space="preserve">LU_cost</t>
   </si>
   <si>
     <t xml:space="preserve">€</t>
   </si>
   <si>
-    <t xml:space="preserve">HA.cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC.cost</t>
+    <t xml:space="preserve">HA_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC_cost</t>
   </si>
   <si>
     <t xml:space="preserve">Int_Out_Flow</t>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">11,8% Energy transformation efficiency from wind to electricity</t>
   </si>
   <si>
-    <t xml:space="preserve">WindElectricity.max_production</t>
+    <t xml:space="preserve">WindElectricity_max_production</t>
   </si>
   <si>
     <t xml:space="preserve">40% capacity factor</t>
@@ -429,7 +429,7 @@
     <t xml:space="preserve">MWh</t>
   </si>
   <si>
-    <t xml:space="preserve">GridElectricity.cost</t>
+    <t xml:space="preserve">GridElectricity_cost</t>
   </si>
   <si>
     <t xml:space="preserve">Env_In_Flow</t>
@@ -456,10 +456,10 @@
     <t xml:space="preserve">DesalinatedWater</t>
   </si>
   <si>
-    <t xml:space="preserve">DesalinatedWater.cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DesalinatedWater.max_production</t>
+    <t xml:space="preserve">DesalinatedWater_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DesalinatedWater_max_production</t>
   </si>
   <si>
     <t xml:space="preserve">40% utilization factor</t>
@@ -486,7 +486,7 @@
     <t xml:space="preserve">From desalination</t>
   </si>
   <si>
-    <t xml:space="preserve">BlueWater.cost</t>
+    <t xml:space="preserve">BlueWater_cost</t>
   </si>
   <si>
     <t xml:space="preserve">Meuro</t>
@@ -498,7 +498,7 @@
     <t xml:space="preserve">Tm</t>
   </si>
   <si>
-    <t xml:space="preserve">Agrochemicals.cost</t>
+    <t xml:space="preserve">Agrochemicals_cost</t>
   </si>
   <si>
     <t xml:space="preserve">Euro</t>
@@ -513,7 +513,7 @@
     <t xml:space="preserve">Pumped from aquifers</t>
   </si>
   <si>
-    <t xml:space="preserve">GreenWater.cost</t>
+    <t xml:space="preserve">GreenWater_cost</t>
   </si>
   <si>
     <t xml:space="preserve">MaterialWastes</t>
@@ -522,7 +522,7 @@
     <t xml:space="preserve">DiffusivePollution</t>
   </si>
   <si>
-    <t xml:space="preserve">Vegetables.cost</t>
+    <t xml:space="preserve">Vegetables_cost</t>
   </si>
   <si>
     <t xml:space="preserve">N-2</t>
@@ -724,18 +724,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65536"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="13.2295918367347"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="13.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,7 +896,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -911,17 +911,17 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="13.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,7 +1025,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1038,25 +1038,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J65536"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.9030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.6632653061225"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,7 +1536,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1551,28 +1551,28 @@
   </sheetPr>
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="13.2295918367347"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="13.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1894,7 +1894,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1909,28 +1909,28 @@
   </sheetPr>
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="15.1173469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="15.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2421,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2436,28 +2436,28 @@
   </sheetPr>
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="13.2295918367347"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="13.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2986,7 +2986,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3001,28 +3001,28 @@
   </sheetPr>
   <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C98" activeCellId="0" sqref="C98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="13.2295918367347"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="13.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6193,7 +6193,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Packages refactoring, ETL improved, new PartialRetrievalDictionary, Eurostat read bulk files modified, new FADN support, many to many mapping, new REST functions, (Workspace - Concepts Helper - Serialization - Data Input - Manager) Improved Incorporates minified version of NIS frontend.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/Soslaires.xlsx
+++ b/backend_tests/z_input_files/Soslaires.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="152">
   <si>
     <t xml:space="preserve">Case study code</t>
   </si>
@@ -314,7 +314,7 @@
     <t xml:space="preserve">ASSESSMENT</t>
   </si>
   <si>
-    <t xml:space="preserve">PEDIGREE TEMPLATE</t>
+    <t xml:space="preserve">PEDIGREE MATRIX</t>
   </si>
   <si>
     <t xml:space="preserve">PEDIGREE</t>
@@ -405,10 +405,6 @@
   </si>
   <si>
     <t xml:space="preserve">0.429 M€ income from energy sale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIGREE
-TEMPLATE</t>
   </si>
   <si>
     <t xml:space="preserve">DesalinationPlant</t>
@@ -535,7 +531,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -586,6 +582,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -642,7 +644,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -703,6 +705,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -726,8 +732,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1056,7 +1062,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,8 +1557,8 @@
   </sheetPr>
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1562,11 +1568,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.08"/>
@@ -1910,7 +1916,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1927,13 +1933,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="15.12"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
@@ -1961,8 +1967,8 @@
       <c r="I1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>113</v>
+      <c r="J1" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>83</v>
@@ -1988,7 +1994,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>90</v>
@@ -2023,7 +2029,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>90</v>
@@ -2050,7 +2056,7 @@
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q3" s="14"/>
       <c r="R3" s="14"/>
@@ -2058,7 +2064,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>90</v>
@@ -2085,7 +2091,7 @@
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
@@ -2093,7 +2099,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>90</v>
@@ -2129,7 +2135,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>90</v>
@@ -2162,7 +2168,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>90</v>
@@ -2195,13 +2201,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>104</v>
@@ -2224,7 +2230,7 @@
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q8" s="14"/>
       <c r="R8" s="14"/>
@@ -2232,13 +2238,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>111</v>
@@ -2247,27 +2253,27 @@
         <v>929</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L9" s="13" t="s">
         <v>96</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" s="8" t="n">
         <v>74000</v>
@@ -2282,22 +2288,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="E11" s="8" t="n">
         <v>1.75</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L11" s="13" t="s">
         <v>96</v>
@@ -2306,42 +2312,42 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="E12" s="8" t="n">
         <v>1.05</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L12" s="13" t="s">
         <v>96</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
@@ -2352,7 +2358,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>90</v>
@@ -2361,20 +2367,20 @@
         <v>103</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E14" s="8" t="n">
         <v>0.7</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L14" s="13"/>
       <c r="P14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>90</v>
@@ -2383,7 +2389,7 @@
         <v>103</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E15" s="8" t="n">
         <v>560000</v>
@@ -2396,7 +2402,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>90</v>
@@ -2405,17 +2411,17 @@
         <v>103</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E16" s="8" t="n">
         <v>1.78</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L16" s="13"/>
       <c r="P16" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2437,7 +2443,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2446,21 +2452,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="13.23"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
@@ -2488,8 +2494,8 @@
       <c r="I1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>113</v>
+      <c r="J1" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>83</v>
@@ -2530,7 +2536,7 @@
         <v>282</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -2598,7 +2604,7 @@
         <v>16.8</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -2625,11 +2631,11 @@
         <v>91</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -2658,7 +2664,7 @@
         <v>91</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="8"/>
@@ -2684,16 +2690,16 @@
         <v>90</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="13" t="n">
         <v>0.67</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -2707,7 +2713,7 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
@@ -2721,16 +2727,16 @@
         <v>90</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="13" t="n">
         <v>0.56</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -2759,13 +2765,13 @@
         <v>110</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" s="13" t="n">
         <v>421</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -2794,13 +2800,13 @@
         <v>110</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E10" s="8" t="n">
         <v>84000</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L10" s="13" t="s">
         <v>96</v>
@@ -2818,7 +2824,7 @@
         <v>110</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -2835,22 +2841,22 @@
         <v>90</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="8" t="n">
         <v>1.48</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L12" s="13" t="s">
         <v>96</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2861,16 +2867,16 @@
         <v>90</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E13" s="8" t="n">
         <v>0.815</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L13" s="13" t="s">
         <v>96</v>
@@ -2884,14 +2890,14 @@
         <v>90</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E14" s="0"/>
       <c r="F14" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>96</v>
@@ -2905,10 +2911,10 @@
         <v>90</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
@@ -2924,14 +2930,14 @@
         <v>90</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L16" s="13" t="s">
         <v>96</v>
@@ -2954,7 +2960,7 @@
         <v>24000</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>96</v>
@@ -2971,13 +2977,13 @@
         <v>103</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E18" s="8" t="n">
         <v>18.3</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L18" s="13" t="s">
         <v>96</v>
@@ -3002,7 +3008,7 @@
   <dimension ref="A1:S97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C98" activeCellId="0" sqref="C98"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3025,7 +3031,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="13.23"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
@@ -3053,8 +3059,8 @@
       <c r="I1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>113</v>
+      <c r="J1" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>83</v>
@@ -3083,7 +3089,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>91</v>
@@ -3095,7 +3101,7 @@
         <v>120</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -3116,7 +3122,7 @@
         <v>34</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>91</v>
@@ -3151,17 +3157,17 @@
         <v>34</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -3184,13 +3190,13 @@
         <v>34</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="8"/>
@@ -3213,19 +3219,19 @@
         <v>34</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E6" s="15" t="n">
+        <v>136</v>
+      </c>
+      <c r="E6" s="16" t="n">
         <v>0.72</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -3239,7 +3245,7 @@
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
@@ -3250,19 +3256,19 @@
         <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="13" t="n">
         <v>116</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -3285,13 +3291,13 @@
         <v>34</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
@@ -3316,17 +3322,17 @@
         <v>34</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
@@ -3349,17 +3355,17 @@
         <v>34</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10" s="0"/>
       <c r="F10" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
@@ -3382,13 +3388,13 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -3413,17 +3419,17 @@
         <v>34</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E12" s="0"/>
       <c r="F12" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
@@ -3446,7 +3452,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>103</v>
@@ -3458,7 +3464,7 @@
         <v>7200</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
@@ -3481,7 +3487,7 @@
         <v>35</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>91</v>
@@ -3493,7 +3499,7 @@
         <v>60</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -3514,7 +3520,7 @@
         <v>35</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>91</v>
@@ -3549,17 +3555,17 @@
         <v>35</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -3582,13 +3588,13 @@
         <v>35</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="8"/>
@@ -3611,19 +3617,19 @@
         <v>35</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18" s="13" t="n">
         <v>0.42</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -3637,7 +3643,7 @@
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
@@ -3648,19 +3654,19 @@
         <v>35</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19" s="13" t="n">
         <v>90</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -3683,13 +3689,13 @@
         <v>35</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
@@ -3714,17 +3720,17 @@
         <v>35</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G21" s="0"/>
       <c r="H21" s="0"/>
@@ -3747,17 +3753,17 @@
         <v>35</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E22" s="0"/>
       <c r="F22" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
@@ -3780,13 +3786,13 @@
         <v>35</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23" s="0"/>
       <c r="F23" s="0"/>
@@ -3811,17 +3817,17 @@
         <v>35</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E24" s="0"/>
       <c r="F24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
@@ -3844,7 +3850,7 @@
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>103</v>
@@ -3856,7 +3862,7 @@
         <v>7800</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G25" s="0"/>
       <c r="H25" s="0"/>
@@ -3879,7 +3885,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>91</v>
@@ -3891,7 +3897,7 @@
         <v>15</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -3912,7 +3918,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>91</v>
@@ -3947,17 +3953,17 @@
         <v>37</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
@@ -3980,13 +3986,13 @@
         <v>37</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="8"/>
@@ -4009,19 +4015,19 @@
         <v>37</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E30" s="13" t="n">
         <v>90000</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
@@ -4035,7 +4041,7 @@
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
       <c r="P30" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
@@ -4046,19 +4052,19 @@
         <v>37</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E31" s="13" t="n">
         <v>22</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -4081,13 +4087,13 @@
         <v>37</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
@@ -4112,17 +4118,17 @@
         <v>37</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
@@ -4145,17 +4151,17 @@
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E34" s="0"/>
       <c r="F34" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G34" s="0"/>
       <c r="H34" s="0"/>
@@ -4178,13 +4184,13 @@
         <v>37</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E35" s="0"/>
       <c r="F35" s="0"/>
@@ -4209,17 +4215,17 @@
         <v>37</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E36" s="0"/>
       <c r="F36" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G36" s="0"/>
       <c r="H36" s="0"/>
@@ -4242,7 +4248,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>103</v>
@@ -4254,7 +4260,7 @@
         <v>1350</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G37" s="0"/>
       <c r="H37" s="0"/>
@@ -4277,7 +4283,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>91</v>
@@ -4289,7 +4295,7 @@
         <v>20</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -4310,7 +4316,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>91</v>
@@ -4345,17 +4351,17 @@
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E40" s="13"/>
       <c r="F40" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -4378,13 +4384,13 @@
         <v>38</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="8"/>
@@ -4407,19 +4413,19 @@
         <v>38</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E42" s="13" t="n">
         <v>0.18</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
@@ -4433,7 +4439,7 @@
       <c r="N42" s="8"/>
       <c r="O42" s="8"/>
       <c r="P42" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
@@ -4444,19 +4450,19 @@
         <v>38</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E43" s="13" t="n">
         <v>62</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
@@ -4479,13 +4485,13 @@
         <v>38</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
@@ -4510,17 +4516,17 @@
         <v>38</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G45" s="0"/>
       <c r="H45" s="0"/>
@@ -4543,17 +4549,17 @@
         <v>38</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E46" s="0"/>
       <c r="F46" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G46" s="0"/>
       <c r="H46" s="0"/>
@@ -4576,13 +4582,13 @@
         <v>38</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E47" s="0"/>
       <c r="F47" s="0"/>
@@ -4607,17 +4613,17 @@
         <v>38</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E48" s="0"/>
       <c r="F48" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G48" s="0"/>
       <c r="H48" s="0"/>
@@ -4640,7 +4646,7 @@
         <v>38</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>103</v>
@@ -4652,7 +4658,7 @@
         <v>3600</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G49" s="0"/>
       <c r="H49" s="0"/>
@@ -4675,7 +4681,7 @@
         <v>39</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>91</v>
@@ -4687,7 +4693,7 @@
         <v>20</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
@@ -4708,7 +4714,7 @@
         <v>39</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>91</v>
@@ -4743,17 +4749,17 @@
         <v>39</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E52" s="13"/>
       <c r="F52" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
@@ -4776,13 +4782,13 @@
         <v>39</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E53" s="13"/>
       <c r="F53" s="8"/>
@@ -4805,19 +4811,19 @@
         <v>39</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E54" s="13" t="n">
         <v>0.21</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
@@ -4831,7 +4837,7 @@
       <c r="N54" s="8"/>
       <c r="O54" s="8"/>
       <c r="P54" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q54" s="8"/>
       <c r="R54" s="8"/>
@@ -4842,19 +4848,19 @@
         <v>39</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E55" s="13" t="n">
         <v>74.6</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
@@ -4877,13 +4883,13 @@
         <v>39</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
@@ -4908,17 +4914,17 @@
         <v>39</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G57" s="0"/>
       <c r="H57" s="0"/>
@@ -4941,17 +4947,17 @@
         <v>39</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E58" s="0"/>
       <c r="F58" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G58" s="0"/>
       <c r="H58" s="0"/>
@@ -4974,13 +4980,13 @@
         <v>39</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
@@ -5005,17 +5011,17 @@
         <v>39</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E60" s="0"/>
       <c r="F60" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G60" s="0"/>
       <c r="H60" s="0"/>
@@ -5038,7 +5044,7 @@
         <v>39</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>103</v>
@@ -5050,7 +5056,7 @@
         <v>1800</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G61" s="0"/>
       <c r="H61" s="0"/>
@@ -5073,7 +5079,7 @@
         <v>40</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>91</v>
@@ -5085,7 +5091,7 @@
         <v>25</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
@@ -5106,7 +5112,7 @@
         <v>40</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>91</v>
@@ -5141,17 +5147,17 @@
         <v>40</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E64" s="13"/>
       <c r="F64" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
@@ -5174,13 +5180,13 @@
         <v>40</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E65" s="13"/>
       <c r="F65" s="8"/>
@@ -5203,19 +5209,19 @@
         <v>40</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E66" s="13" t="n">
         <v>0.1</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
@@ -5229,7 +5235,7 @@
       <c r="N66" s="8"/>
       <c r="O66" s="8"/>
       <c r="P66" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q66" s="8"/>
       <c r="R66" s="8"/>
@@ -5240,19 +5246,19 @@
         <v>40</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E67" s="13" t="n">
         <v>31</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
@@ -5275,13 +5281,13 @@
         <v>40</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E68" s="0"/>
       <c r="F68" s="0"/>
@@ -5306,17 +5312,17 @@
         <v>40</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G69" s="0"/>
       <c r="H69" s="0"/>
@@ -5339,17 +5345,17 @@
         <v>40</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E70" s="0"/>
       <c r="F70" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G70" s="0"/>
       <c r="H70" s="0"/>
@@ -5372,13 +5378,13 @@
         <v>40</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E71" s="0"/>
       <c r="F71" s="0"/>
@@ -5403,17 +5409,17 @@
         <v>40</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E72" s="0"/>
       <c r="F72" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G72" s="0"/>
       <c r="H72" s="0"/>
@@ -5436,7 +5442,7 @@
         <v>40</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>103</v>
@@ -5448,7 +5454,7 @@
         <v>2250</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G73" s="0"/>
       <c r="H73" s="0"/>
@@ -5471,7 +5477,7 @@
         <v>41</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>91</v>
@@ -5483,7 +5489,7 @@
         <v>15</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -5504,7 +5510,7 @@
         <v>41</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>91</v>
@@ -5539,17 +5545,17 @@
         <v>41</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E76" s="13"/>
       <c r="F76" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
@@ -5572,13 +5578,13 @@
         <v>41</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="8"/>
@@ -5601,19 +5607,19 @@
         <v>41</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E78" s="13" t="n">
         <v>0.18</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
@@ -5627,7 +5633,7 @@
       <c r="N78" s="8"/>
       <c r="O78" s="8"/>
       <c r="P78" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q78" s="8"/>
       <c r="R78" s="8"/>
@@ -5638,19 +5644,19 @@
         <v>41</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E79" s="13" t="n">
         <v>26</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
@@ -5673,13 +5679,13 @@
         <v>41</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E80" s="0"/>
       <c r="F80" s="0"/>
@@ -5704,17 +5710,17 @@
         <v>41</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E81" s="8"/>
       <c r="F81" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G81" s="0"/>
       <c r="H81" s="0"/>
@@ -5737,17 +5743,17 @@
         <v>41</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E82" s="0"/>
       <c r="F82" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G82" s="0"/>
       <c r="H82" s="0"/>
@@ -5770,13 +5776,13 @@
         <v>41</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E83" s="0"/>
       <c r="F83" s="0"/>
@@ -5801,17 +5807,17 @@
         <v>41</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E84" s="0"/>
       <c r="F84" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G84" s="0"/>
       <c r="H84" s="0"/>
@@ -5834,7 +5840,7 @@
         <v>41</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>103</v>
@@ -5846,7 +5852,7 @@
         <v>113</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G85" s="0"/>
       <c r="H85" s="0"/>
@@ -5869,7 +5875,7 @@
         <v>42</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>91</v>
@@ -5881,7 +5887,7 @@
         <v>7</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
@@ -5902,7 +5908,7 @@
         <v>42</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>91</v>
@@ -5937,17 +5943,17 @@
         <v>42</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E88" s="13"/>
       <c r="F88" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
@@ -5970,13 +5976,13 @@
         <v>42</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>91</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E89" s="13"/>
       <c r="F89" s="8"/>
@@ -5999,19 +6005,19 @@
         <v>42</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E90" s="13" t="n">
         <v>0.25</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
@@ -6025,7 +6031,7 @@
       <c r="N90" s="8"/>
       <c r="O90" s="8"/>
       <c r="P90" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q90" s="8"/>
       <c r="R90" s="8"/>
@@ -6036,17 +6042,17 @@
         <v>42</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E91" s="13"/>
       <c r="F91" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
@@ -6069,13 +6075,13 @@
         <v>42</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E92" s="0"/>
       <c r="F92" s="0"/>
@@ -6089,17 +6095,17 @@
         <v>42</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E93" s="8"/>
       <c r="F93" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L93" s="13" t="s">
         <v>96</v>
@@ -6111,17 +6117,17 @@
         <v>42</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E94" s="0"/>
       <c r="F94" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L94" s="13" t="s">
         <v>96</v>
@@ -6132,13 +6138,13 @@
         <v>42</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E95" s="0"/>
       <c r="F95" s="0"/>
@@ -6151,17 +6157,17 @@
         <v>42</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E96" s="0"/>
       <c r="F96" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L96" s="13" t="s">
         <v>96</v>
@@ -6172,7 +6178,7 @@
         <v>42</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>103</v>
@@ -6184,7 +6190,7 @@
         <v>56</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L97" s="13" t="s">
         <v>96</v>

</xml_diff>